<commit_message>
Support channel ID YouTube URLs, custom Substack domains, and add xlsx-to-json script
Fix YouTube fetching to handle /channel/ URLs directly without handle
lookup. Fix Substack RSS to work with any domain, not just *.substack.com.
Add scripts/xlsx-to-json.js for syncing spreadsheet data to data.json.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/IndependentVoicesData.xlsx
+++ b/IndependentVoicesData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flinn\bias-database-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4318A4-18F9-4AE1-8244-37EA08DE22E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AD31D8-752B-44A2-A4E8-B4C98709E668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="915" windowWidth="29310" windowHeight="19770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8835" yWindow="345" windowWidth="29310" windowHeight="19770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Independent Voices Bias Databas" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="449">
   <si>
     <t>Individual</t>
   </si>
@@ -1346,6 +1346,30 @@
   </si>
   <si>
     <t>https://www.tiktok.com/@aaronparnas1?lang=en</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/officialbenshapiro</t>
+  </si>
+  <si>
+    <t>https://x.com/benshapiro</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCnQC_G5Xsjhp9fEJKuIcrSw</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@real.benshapiro?lang=en</t>
+  </si>
+  <si>
+    <t>https://www.noahpinion.blog/</t>
+  </si>
+  <si>
+    <t>https://x.com/Noahpinion</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@ECON102Podcast</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1499,6 +1523,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1722,8 +1749,8 @@
   </sheetPr>
   <dimension ref="A1:AA998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1733,6 +1760,10 @@
     <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1872,11 +1903,21 @@
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>445</v>
+      </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -1905,11 +1946,21 @@
       <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>444</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -25718,6 +25769,7 @@
     <hyperlink ref="G3" r:id="rId2" xr:uid="{E3B29146-C01F-4D88-907F-8E0EF9095B5F}"/>
     <hyperlink ref="H3" r:id="rId3" xr:uid="{00B2EE1B-1A9B-4334-BD0F-B45BCA2C0C7E}"/>
     <hyperlink ref="I3" r:id="rId4" xr:uid="{9AFBF6A4-7FBB-409E-9259-CA6815120743}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{846B1A20-8C7D-4DF1-8C1F-E54FFCB1F2C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add social media URLs for commentators
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/IndependentVoicesData.xlsx
+++ b/IndependentVoicesData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flinn\bias-database-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AD31D8-752B-44A2-A4E8-B4C98709E668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6710D1-D27A-4876-8EFE-3BB3DEB0A394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8835" yWindow="345" windowWidth="29310" windowHeight="19770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="345" windowWidth="37845" windowHeight="19770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Independent Voices Bias Databas" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="547">
   <si>
     <t>Individual</t>
   </si>
@@ -145,21 +145,9 @@
     <t>Policy professionals, moderate Democrats, and "YIMBY" (Yes In My Backyard) advocates.</t>
   </si>
   <si>
-    <t>Bari Weiss</t>
-  </si>
-  <si>
     <t>15R</t>
   </si>
   <si>
-    <t>Liberalism (in the classical sense), free speech, and opposition to "illiberalism" on the left.</t>
-  </si>
-  <si>
-    <t>Cancel culture, anti-Semitism, and the "capture" of elite institutions by progressive ideology.</t>
-  </si>
-  <si>
-    <t>Disaffected liberals, "intellectual dark web" fans, and centrist conservatives.</t>
-  </si>
-  <si>
     <t>Lee Fang</t>
   </si>
   <si>
@@ -1370,13 +1358,319 @@
   </si>
   <si>
     <t>https://www.youtube.com/@ECON102Podcast</t>
+  </si>
+  <si>
+    <t>https://x.com/nickshirleyy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@NickShirley</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/nickshirley</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@nickshirleyy</t>
+  </si>
+  <si>
+    <t>https://x.com/Channel5iveNews</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@Channel5YouTube</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/andreww.me</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@channel5andrewcallaghan</t>
+  </si>
+  <si>
+    <t>https://x.com/NateSilver538</t>
+  </si>
+  <si>
+    <t>https://www.natesilver.net</t>
+  </si>
+  <si>
+    <t>https://x.com/mattyglesias</t>
+  </si>
+  <si>
+    <t>https://www.slowboring.com</t>
+  </si>
+  <si>
+    <t>https://x.com/lhfang</t>
+  </si>
+  <si>
+    <t>https://www.leefang.com</t>
+  </si>
+  <si>
+    <t>https://x.com/kylascan</t>
+  </si>
+  <si>
+    <t>https://kyla.substack.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@kylascanlon</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/kylascan</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@kylascan</t>
+  </si>
+  <si>
+    <t>https://x.com/ChrisCillizza</t>
+  </si>
+  <si>
+    <t>https://chriscillizza.substack.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/chriscillizza</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/cillizzac</t>
+  </si>
+  <si>
+    <t>https://x.com/TheOmniLiberal</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@destiny</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/destiny</t>
+  </si>
+  <si>
+    <t>https://x.com/briantylercohen</t>
+  </si>
+  <si>
+    <t>https://plus.briantylercohen.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@briantylercohen</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/briantylercohen</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@briantylercohen</t>
+  </si>
+  <si>
+    <t>https://x.com/HC_Richardson</t>
+  </si>
+  <si>
+    <t>https://heathercoxrichardson.substack.com</t>
+  </si>
+  <si>
+    <t>https://x.com/hasanthehun</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@hasanabi</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/hasandpiker</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@hasandpiker</t>
+  </si>
+  <si>
+    <t>https://x.com/dpakman</t>
+  </si>
+  <si>
+    <t>https://substack.davidpakman.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@thedavidpakmanshow</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/david.pakman</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@davidpakmanshow</t>
+  </si>
+  <si>
+    <t>https://x.com/atrupar</t>
+  </si>
+  <si>
+    <t>https://www.publicnotice.co</t>
+  </si>
+  <si>
+    <t>https://x.com/RBReich</t>
+  </si>
+  <si>
+    <t>https://robertreich.substack.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@RBReich</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/rbreich</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@rbreich</t>
+  </si>
+  <si>
+    <t>https://x.com/kylekulinski</t>
+  </si>
+  <si>
+    <t>https://krystalkyleandfriends.substack.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@SecularTalk</t>
+  </si>
+  <si>
+    <t>https://x.com/contrapoints</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@ContraPoints</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/contrapoints</t>
+  </si>
+  <si>
+    <t>https://x.com/MeidasTouch</t>
+  </si>
+  <si>
+    <t>https://www.meidasplus.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@MeidasTouch</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/meidastouch</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@meidastouch</t>
+  </si>
+  <si>
+    <t>https://x.com/TuckerCarlson</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@TuckerCarlson</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/tuckercarlson</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@tuckercarlson</t>
+  </si>
+  <si>
+    <t>https://x.com/RealCandaceO</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@realcandaceo</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/realcandaceowens</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@candaceoshow</t>
+  </si>
+  <si>
+    <t>https://x.com/Timcast</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@Timcast</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/timcast</t>
+  </si>
+  <si>
+    <t>https://x.com/realchrisrufo</t>
+  </si>
+  <si>
+    <t>https://christopherrufo.com</t>
+  </si>
+  <si>
+    <t>https://x.com/MattWalshBlog</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@MattWalshBlog</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/mattwalshblog</t>
+  </si>
+  <si>
+    <t>https://x.com/KonstantinKisin</t>
+  </si>
+  <si>
+    <t>https://www.konstantinkisin.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@TRIGGERnometry</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/konstantinkisin</t>
+  </si>
+  <si>
+    <t>https://x.com/shellenberger</t>
+  </si>
+  <si>
+    <t>https://public.substack.com</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/shellenberger</t>
+  </si>
+  <si>
+    <t>https://x.com/scrowder</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@StevenCrowder</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/louderwithcrowder</t>
+  </si>
+  <si>
+    <t>https://x.com/EWErickson</t>
+  </si>
+  <si>
+    <t>https://ewerickson.substack.com</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/ewerickson</t>
+  </si>
+  <si>
+    <t>https://x.com/mehdirhasan</t>
+  </si>
+  <si>
+    <t>https://zeteo.com</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@ZeteoNews</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/mehdirhasan</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@mehdirhasan</t>
+  </si>
+  <si>
+    <t>https://x.com/mtaibbi</t>
+  </si>
+  <si>
+    <t>https://www.racket.news</t>
+  </si>
+  <si>
+    <t>https://x.com/tylercowen?lang=en</t>
+  </si>
+  <si>
+    <t>https://substack.com/@tylercowen</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@CowenConvos</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/cowenconvos/?hl=en</t>
+  </si>
+  <si>
+    <t>https://x.com/JuddLegum</t>
+  </si>
+  <si>
+    <t>https://popular.info/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1430,6 +1724,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1486,7 +1786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1527,6 +1827,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1747,10 +2053,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA998"/>
+  <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1760,10 +2066,11 @@
     <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="55.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1783,19 +2090,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>435</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>437</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>436</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>438</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>439</v>
       </c>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -1844,7 +2151,7 @@
       <c r="Z2" s="10"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:27" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1861,19 +2168,19 @@
         <v>9</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
@@ -1904,19 +2211,19 @@
         <v>14</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="I4" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>441</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>445</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -1930,7 +2237,7 @@
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -1947,19 +2254,19 @@
         <v>19</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -1973,7 +2280,7 @@
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
     </row>
-    <row r="6" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1989,11 +2296,21 @@
       <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="F6" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>448</v>
+      </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -2006,7 +2323,7 @@
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
     </row>
-    <row r="7" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -2022,11 +2339,21 @@
       <c r="E7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="F7" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>452</v>
+      </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -2039,7 +2366,7 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -2055,11 +2382,15 @@
       <c r="E8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="F8" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -2072,7 +2403,7 @@
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
@@ -2088,11 +2419,15 @@
       <c r="E9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="F9" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -2105,12 +2440,12 @@
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>42</v>
@@ -2121,11 +2456,15 @@
       <c r="E10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="F10" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -2138,27 +2477,37 @@
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>463</v>
+      </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
@@ -2171,12 +2520,12 @@
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
     </row>
-    <row r="12" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="7" t="s">
         <v>50</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>51</v>
@@ -2187,11 +2536,21 @@
       <c r="E12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="F12" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -2204,12 +2563,12 @@
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="7">
-        <v>0</v>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>55</v>
@@ -2220,11 +2579,17 @@
       <c r="E13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="F13" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="J13" s="16"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -2237,27 +2602,34 @@
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>541</v>
+      </c>
+      <c r="G14" t="s">
+        <v>542</v>
+      </c>
+      <c r="H14" t="s">
+        <v>543</v>
+      </c>
+      <c r="I14" t="s">
+        <v>544</v>
+      </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -2270,27 +2642,28 @@
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="7" t="s">
         <v>63</v>
       </c>
+      <c r="B15" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="C15" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="F15" t="s">
+        <v>545</v>
+      </c>
+      <c r="G15" t="s">
+        <v>546</v>
+      </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -2303,27 +2676,37 @@
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>472</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>473</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>475</v>
+      </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
@@ -2336,27 +2719,37 @@
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
     </row>
-    <row r="17" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -2369,27 +2762,37 @@
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
     </row>
-    <row r="18" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+        <v>82</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>478</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>481</v>
+      </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
@@ -2402,12 +2805,12 @@
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
     </row>
-    <row r="19" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>84</v>
@@ -2418,11 +2821,21 @@
       <c r="E19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="F19" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>486</v>
+      </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
@@ -2435,27 +2848,37 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>488</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
@@ -2468,12 +2891,12 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>93</v>
@@ -2484,11 +2907,21 @@
       <c r="E21" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="F21" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>493</v>
+      </c>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
@@ -2501,12 +2934,12 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>97</v>
@@ -2517,11 +2950,21 @@
       <c r="E22" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
+      <c r="F22" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -2534,27 +2977,37 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
@@ -2567,27 +3020,37 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+        <v>109</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>502</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>503</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>504</v>
+      </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
@@ -2600,27 +3063,37 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B25" s="6" t="s">
         <v>110</v>
       </c>
+      <c r="B25" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="C25" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
+        <v>114</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>508</v>
+      </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
@@ -2633,27 +3106,37 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>510</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>512</v>
+      </c>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -2666,27 +3149,37 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>514</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>440</v>
+      </c>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
@@ -2699,12 +3192,12 @@
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>126</v>
@@ -2715,11 +3208,21 @@
       <c r="E28" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
+      <c r="F28" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
@@ -2732,27 +3235,37 @@
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
     </row>
-    <row r="29" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
+        <v>133</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
@@ -2765,27 +3278,37 @@
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
+        <v>138</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>521</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
@@ -2798,27 +3321,37 @@
       <c r="T30" s="7"/>
       <c r="U30" s="7"/>
     </row>
-    <row r="31" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
+        <v>143</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
@@ -2831,27 +3364,37 @@
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
     </row>
-    <row r="32" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
+        <v>148</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>528</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
@@ -2864,12 +3407,12 @@
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>
     </row>
-    <row r="33" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>150</v>
@@ -2880,11 +3423,21 @@
       <c r="E33" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
+      <c r="F33" s="16" t="s">
+        <v>531</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>533</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
@@ -2897,12 +3450,12 @@
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
     </row>
-    <row r="34" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>21</v>
+      <c r="B34" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>154</v>
@@ -2913,11 +3466,21 @@
       <c r="E34" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
+      <c r="F34" s="16" t="s">
+        <v>534</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>538</v>
+      </c>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
@@ -2930,12 +3493,12 @@
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>73</v>
+      <c r="B35" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>158</v>
@@ -2946,11 +3509,21 @@
       <c r="E35" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
+      <c r="F35" s="16" t="s">
+        <v>539</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>540</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>440</v>
+      </c>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
@@ -2967,17 +3540,17 @@
       <c r="A36" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>41</v>
+      <c r="B36" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -2998,19 +3571,19 @@
     </row>
     <row r="37" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -3031,10 +3604,10 @@
     </row>
     <row r="38" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>171</v>
+        <v>6</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>172</v>
@@ -3066,17 +3639,17 @@
       <c r="A39" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>6</v>
+      <c r="B39" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
@@ -3097,10 +3670,10 @@
     </row>
     <row r="40" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B40" s="7" t="s">
         <v>180</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>181</v>
@@ -3133,7 +3706,7 @@
         <v>184</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>185</v>
@@ -3166,7 +3739,7 @@
         <v>188</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>189</v>
@@ -3199,7 +3772,7 @@
         <v>192</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>193</v>
@@ -3227,12 +3800,12 @@
       <c r="T43" s="7"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="44" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>196</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>197</v>
@@ -3260,12 +3833,12 @@
       <c r="T44" s="7"/>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>200</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>201</v>
@@ -3298,9 +3871,9 @@
         <v>204</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>205</v>
       </c>
       <c r="D46" s="5" t="s">
@@ -3331,9 +3904,9 @@
         <v>208</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>209</v>
       </c>
       <c r="D47" s="5" t="s">
@@ -3363,17 +3936,17 @@
       <c r="A48" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>83</v>
+      <c r="B48" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
@@ -3394,10 +3967,10 @@
     </row>
     <row r="49" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>217</v>
+        <v>111</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>218</v>
@@ -3430,16 +4003,16 @@
         <v>221</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>115</v>
+        <v>222</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -3458,12 +4031,12 @@
       <c r="T50" s="7"/>
       <c r="U50" s="7"/>
     </row>
-    <row r="51" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B51" s="8" t="s">
         <v>226</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>227</v>
@@ -3491,21 +4064,21 @@
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>230</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>73</v>
+        <v>231</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
@@ -3526,10 +4099,10 @@
     </row>
     <row r="53" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B53" s="6" t="s">
         <v>235</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>236</v>
@@ -3559,19 +4132,19 @@
     </row>
     <row r="54" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C54" s="5" t="s">
+      <c r="D54" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>242</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
@@ -3592,19 +4165,19 @@
     </row>
     <row r="55" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>36</v>
+        <v>394</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="C55" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>245</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
@@ -3625,19 +4198,19 @@
     </row>
     <row r="56" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>398</v>
+        <v>245</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>166</v>
+        <v>246</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
@@ -3658,19 +4231,19 @@
     </row>
     <row r="57" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B57" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="D57" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>251</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>253</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
@@ -3691,19 +4264,19 @@
     </row>
     <row r="58" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>26</v>
+        <v>396</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="C58" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
@@ -3722,21 +4295,21 @@
       <c r="T58" s="7"/>
       <c r="U58" s="7"/>
     </row>
-    <row r="59" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>68</v>
+        <v>255</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
@@ -3755,9 +4328,9 @@
       <c r="T59" s="7"/>
       <c r="U59" s="7"/>
     </row>
-    <row r="60" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>259</v>
+        <v>397</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>260</v>
@@ -3788,21 +4361,21 @@
       <c r="T60" s="7"/>
       <c r="U60" s="7"/>
     </row>
-    <row r="61" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="B61" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="D61" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="E61" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
@@ -3821,12 +4394,12 @@
       <c r="T61" s="7"/>
       <c r="U61" s="7"/>
     </row>
-    <row r="62" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>92</v>
+        <v>267</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>268</v>
@@ -3856,19 +4429,19 @@
     </row>
     <row r="63" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>403</v>
+        <v>184</v>
       </c>
       <c r="B63" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="D63" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="E63" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
@@ -3889,10 +4462,10 @@
     </row>
     <row r="64" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>188</v>
+        <v>400</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>110</v>
+        <v>274</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>275</v>
@@ -3922,19 +4495,19 @@
     </row>
     <row r="65" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B65" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="D65" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
@@ -3955,19 +4528,19 @@
     </row>
     <row r="66" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>105</v>
+        <v>402</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="C66" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>284</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
@@ -3988,19 +4561,19 @@
     </row>
     <row r="67" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>264</v>
+        <v>403</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C67" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>287</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
@@ -4021,19 +4594,19 @@
     </row>
     <row r="68" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C68" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
@@ -4054,19 +4627,19 @@
     </row>
     <row r="69" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>73</v>
+        <v>405</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C69" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="E69" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>293</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
@@ -4087,19 +4660,19 @@
     </row>
     <row r="70" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C70" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="E70" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>296</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
@@ -4118,21 +4691,21 @@
       <c r="T70" s="7"/>
       <c r="U70" s="7"/>
     </row>
-    <row r="71" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="C71" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
@@ -4151,12 +4724,12 @@
       <c r="T71" s="7"/>
       <c r="U71" s="7"/>
     </row>
-    <row r="72" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>264</v>
+        <v>299</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>300</v>
@@ -4186,19 +4759,19 @@
     </row>
     <row r="73" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B73" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C73" s="5" t="s">
+      <c r="D73" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="E73" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>306</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
@@ -4219,19 +4792,19 @@
     </row>
     <row r="74" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>165</v>
+        <v>408</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>166</v>
+        <v>69</v>
       </c>
       <c r="C74" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="E74" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>309</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
@@ -4252,19 +4825,19 @@
     </row>
     <row r="75" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>412</v>
+        <v>309</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>73</v>
+        <v>310</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
@@ -4285,19 +4858,19 @@
     </row>
     <row r="76" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="B76" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="D76" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="E76" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>317</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -4318,10 +4891,10 @@
     </row>
     <row r="77" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>260</v>
+        <v>317</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>318</v>
@@ -4349,21 +4922,21 @@
       <c r="T77" s="7"/>
       <c r="U77" s="7"/>
     </row>
-    <row r="78" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="B78" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" s="5" t="s">
+      <c r="D78" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="E78" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>324</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
@@ -4382,12 +4955,12 @@
       <c r="T78" s="7"/>
       <c r="U78" s="7"/>
     </row>
-    <row r="79" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>26</v>
+        <v>324</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>325</v>
@@ -4417,10 +4990,10 @@
     </row>
     <row r="80" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>328</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>329</v>
@@ -4450,19 +5023,19 @@
     </row>
     <row r="81" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B81" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="D81" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="E81" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>335</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
@@ -4483,19 +5056,19 @@
     </row>
     <row r="82" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>83</v>
+        <v>421</v>
+      </c>
+      <c r="B82" s="7">
+        <v>0</v>
       </c>
       <c r="C82" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="E82" s="5" t="s">
         <v>337</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>338</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
@@ -4516,19 +5089,19 @@
     </row>
     <row r="83" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="B83" s="7">
-        <v>0</v>
+        <v>125</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C83" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>340</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>341</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
@@ -4549,10 +5122,10 @@
     </row>
     <row r="84" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>11</v>
+        <v>341</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>342</v>
@@ -4582,19 +5155,19 @@
     </row>
     <row r="85" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C85" s="5" t="s">
+      <c r="D85" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="E85" s="5" t="s">
         <v>347</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>348</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
@@ -4615,19 +5188,19 @@
     </row>
     <row r="86" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="C86" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="D86" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="E86" s="5" t="s">
         <v>350</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>351</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
@@ -4646,21 +5219,21 @@
       <c r="T86" s="7"/>
       <c r="U86" s="7"/>
     </row>
-    <row r="87" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C87" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="E87" s="5" t="s">
         <v>353</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>354</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
@@ -4679,21 +5252,21 @@
       <c r="T87" s="7"/>
       <c r="U87" s="7"/>
     </row>
-    <row r="88" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="C88" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="E88" s="5" t="s">
         <v>356</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>357</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
@@ -4714,19 +5287,19 @@
     </row>
     <row r="89" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="C89" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="E89" s="5" t="s">
         <v>359</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>360</v>
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
@@ -4747,19 +5320,19 @@
     </row>
     <row r="90" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C90" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" s="5" t="s">
         <v>362</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>363</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
@@ -4778,21 +5351,21 @@
       <c r="T90" s="7"/>
       <c r="U90" s="7"/>
     </row>
-    <row r="91" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C91" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="E91" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>366</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -4811,21 +5384,21 @@
       <c r="T91" s="7"/>
       <c r="U91" s="7"/>
     </row>
-    <row r="92" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>83</v>
+        <v>246</v>
       </c>
       <c r="C92" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="E92" s="5" t="s">
         <v>368</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>369</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
@@ -4846,19 +5419,19 @@
     </row>
     <row r="93" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="C93" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="E93" s="5" t="s">
         <v>371</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>372</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
@@ -4877,12 +5450,12 @@
       <c r="T93" s="7"/>
       <c r="U93" s="7"/>
     </row>
-    <row r="94" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>278</v>
+        <v>411</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>372</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>373</v>
@@ -4910,21 +5483,21 @@
       <c r="T94" s="7"/>
       <c r="U94" s="7"/>
     </row>
-    <row r="95" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="B95" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="D95" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="E95" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>379</v>
       </c>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
@@ -4945,10 +5518,10 @@
     </row>
     <row r="96" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>380</v>
@@ -4976,21 +5549,21 @@
       <c r="T96" s="7"/>
       <c r="U96" s="7"/>
     </row>
-    <row r="97" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C97" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="B97" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C97" s="5" t="s">
+      <c r="D97" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="E97" s="5" t="s">
         <v>385</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>386</v>
       </c>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
@@ -5009,21 +5582,21 @@
       <c r="T97" s="7"/>
       <c r="U97" s="7"/>
     </row>
-    <row r="98" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:21" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>125</v>
+        <v>426</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="C98" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="D98" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="E98" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>389</v>
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
@@ -5042,12 +5615,12 @@
       <c r="T98" s="7"/>
       <c r="U98" s="7"/>
     </row>
-    <row r="99" spans="1:21" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
-        <v>430</v>
+        <v>389</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>264</v>
+        <v>69</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>390</v>
@@ -5075,22 +5648,12 @@
       <c r="T99" s="7"/>
       <c r="U99" s="7"/>
     </row>
-    <row r="100" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A100" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>396</v>
-      </c>
+    <row r="100" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A100" s="5"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
@@ -25739,29 +26302,6 @@
       <c r="T997" s="7"/>
       <c r="U997" s="7"/>
     </row>
-    <row r="998" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A998" s="5"/>
-      <c r="B998" s="7"/>
-      <c r="C998" s="5"/>
-      <c r="D998" s="5"/>
-      <c r="E998" s="5"/>
-      <c r="F998" s="7"/>
-      <c r="G998" s="7"/>
-      <c r="H998" s="7"/>
-      <c r="I998" s="7"/>
-      <c r="J998" s="7"/>
-      <c r="K998" s="7"/>
-      <c r="L998" s="7"/>
-      <c r="M998" s="7"/>
-      <c r="N998" s="7"/>
-      <c r="O998" s="7"/>
-      <c r="P998" s="7"/>
-      <c r="Q998" s="7"/>
-      <c r="R998" s="7"/>
-      <c r="S998" s="7"/>
-      <c r="T998" s="7"/>
-      <c r="U998" s="7"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:U1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
@@ -25770,7 +26310,41 @@
     <hyperlink ref="H3" r:id="rId3" xr:uid="{00B2EE1B-1A9B-4334-BD0F-B45BCA2C0C7E}"/>
     <hyperlink ref="I3" r:id="rId4" xr:uid="{9AFBF6A4-7FBB-409E-9259-CA6815120743}"/>
     <hyperlink ref="I4" r:id="rId5" xr:uid="{846B1A20-8C7D-4DF1-8C1F-E54FFCB1F2C4}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{0241C323-3AB5-4B4E-ACC4-3CC2D262B1A8}"/>
+    <hyperlink ref="H6" r:id="rId7" xr:uid="{4D16D180-E491-4A24-AE3C-4ABFBEF93ACA}"/>
+    <hyperlink ref="I6" r:id="rId8" xr:uid="{1681B9FD-3B0E-4448-8218-2EC641CCEE38}"/>
+    <hyperlink ref="J6" r:id="rId9" xr:uid="{4CB0F667-4ED1-4886-BD84-B8586F301DD9}"/>
+    <hyperlink ref="F7" r:id="rId10" xr:uid="{0016F1FF-D98F-4205-A38C-D7875FBD6691}"/>
+    <hyperlink ref="H7" r:id="rId11" xr:uid="{BF26C47F-DD1D-446C-ADAA-183481AF5BB9}"/>
+    <hyperlink ref="I7" r:id="rId12" xr:uid="{891DF46A-B1D8-454C-8B3A-A4521480DA40}"/>
+    <hyperlink ref="J7" r:id="rId13" xr:uid="{71867C35-D4C8-41D7-A4C3-86DB6AA59AEE}"/>
+    <hyperlink ref="F8" r:id="rId14" xr:uid="{E88F3286-9E14-4296-8427-C83373112121}"/>
+    <hyperlink ref="G8" r:id="rId15" display="https://www.natesilver.net/" xr:uid="{AF44960C-6BDA-47FD-A6F7-0F0E271246A6}"/>
+    <hyperlink ref="F9" r:id="rId16" xr:uid="{8B97DF64-992A-4D26-AD37-AF68DE5FC70E}"/>
+    <hyperlink ref="G9" r:id="rId17" display="https://www.slowboring.com/" xr:uid="{A89801B5-6E07-4AB7-8BD3-E6D820D631A8}"/>
+    <hyperlink ref="F10" r:id="rId18" xr:uid="{7E8567C2-FE8C-4E7A-986B-A7849CC7432F}"/>
+    <hyperlink ref="G10" r:id="rId19" display="https://www.leefang.com/" xr:uid="{F94473D1-C6B0-4C85-9DF7-263F417B467A}"/>
+    <hyperlink ref="F11" r:id="rId20" xr:uid="{ACD2E0F8-72DD-4FCB-ADAA-668871FA204B}"/>
+    <hyperlink ref="G11" r:id="rId21" display="https://kyla.substack.com/" xr:uid="{F7C5BD4D-9540-4CED-A182-CF5E19AD0AAB}"/>
+    <hyperlink ref="H11" r:id="rId22" xr:uid="{8192CF19-F9C8-4FCE-8E50-19F280DC1DF5}"/>
+    <hyperlink ref="I11" r:id="rId23" xr:uid="{9CA0240F-25B7-4548-9098-D740881E8C7E}"/>
+    <hyperlink ref="J11" r:id="rId24" xr:uid="{13B3532A-C8DD-4D78-A8EA-990D95DCC352}"/>
+    <hyperlink ref="F12" r:id="rId25" xr:uid="{E536345C-F1AB-4083-A12D-0B9582FB5D42}"/>
+    <hyperlink ref="G12" r:id="rId26" display="https://chriscillizza.substack.com/" xr:uid="{ACB9BF67-DAEF-4741-815E-EAD0409F40DD}"/>
+    <hyperlink ref="H12" r:id="rId27" xr:uid="{3A4D286E-B2EC-4606-9B9D-9873D4BE09A6}"/>
+    <hyperlink ref="I12" r:id="rId28" xr:uid="{47383F10-9C6A-44B6-B236-DB9E111752AF}"/>
+    <hyperlink ref="F13" r:id="rId29" xr:uid="{B2D8CC6E-0A22-457C-868E-801CD384EEE4}"/>
+    <hyperlink ref="H13" r:id="rId30" xr:uid="{EA93EC8C-6089-4417-B73B-1336C3A60F34}"/>
+    <hyperlink ref="I13" r:id="rId31" xr:uid="{D53C4E4C-3E52-4541-AA99-3485C73E0917}"/>
+    <hyperlink ref="F16" r:id="rId32" display="https://x.com/tylercowen" xr:uid="{2D07790E-C787-4E23-86A5-ED09D7819B6B}"/>
+    <hyperlink ref="F17" r:id="rId33" display="https://x.com/JuddLegum" xr:uid="{07D6DBF2-7388-4F45-92B8-31357A23F396}"/>
+    <hyperlink ref="G17" r:id="rId34" display="https://popular.info/" xr:uid="{CE0CFC15-5E1D-4D97-AFC6-A1B889C45535}"/>
+    <hyperlink ref="F27" r:id="rId35" display="https://x.com/TuckerCarlson" xr:uid="{2B234956-E471-43EF-9BA5-B134C88AFE00}"/>
+    <hyperlink ref="H27" r:id="rId36" display="https://www.youtube.com/@tcnetwork" xr:uid="{501A4791-22D2-46AC-AE62-0E0DBADDA791}"/>
+    <hyperlink ref="I27" r:id="rId37" display="https://www.instagram.com/tuckercarlson" xr:uid="{57703EBC-1F3B-48B6-A2D9-032BC57BBDC0}"/>
+    <hyperlink ref="J27" r:id="rId38" display="https://www.tiktok.com/@tuckercarlson" xr:uid="{D88FB67E-1507-4672-A068-F457391003A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>